<commit_message>
Verify Feature #124: TCTO completion date recording
Feature was already fully implemented - verification only task.

Verified functionality:
- Completion date recording with date picker
- Optional repair record linking
- Real-time compliance percentage updates
- Success messages and UI feedback
- Completion info displayed in assets table
- All 3 assets reached 100% compliance

Screenshots captured showing:
- Completion modal with date and repair fields
- Asset compliance updates (33% → 67% → 100%)
- Final state with all assets compliant

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/.playwright-mcp/CUI-PMI-Schedule-20260120.xlsx
+++ b/.playwright-mcp/CUI-PMI-Schedule-20260120.xlsx
@@ -426,7 +426,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Generated: 2026-01-20 00:55:31Z</v>
+        <v>Generated: 2026-01-20 04:03:16Z</v>
       </c>
     </row>
     <row r="5">
@@ -683,10 +683,10 @@
         <v>52III</v>
       </c>
       <c r="G15" t="str">
-        <v>2026-05-19Z</v>
+        <v>2026-05-20Z</v>
       </c>
       <c r="H15" t="str">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I15" t="str">
         <v>-</v>

</xml_diff>